<commit_message>
avances para la carga de trazas
</commit_message>
<xml_diff>
--- a/resources/templates/chas-nacional.xlsx
+++ b/resources/templates/chas-nacional.xlsx
@@ -1,37 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\4 - Proyectos\Moder-Traza-Autopartes\07 - Pruebas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E2EF47B-7D48-478A-A7B5-F9F277196522}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="27320" windowHeight="14900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="DATOS" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Modelo</t>
   </si>
@@ -79,12 +73,15 @@
   </si>
   <si>
     <t>Fotos (IF)</t>
+  </si>
+  <si>
+    <t>Organismo certificador</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -136,14 +133,14 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -151,23 +148,23 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -250,58 +247,58 @@
     </xf>
   </cellXfs>
   <cellStyles count="53">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Hipervínculo visitado" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -638,31 +635,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.25" customWidth="1"/>
-    <col min="14" max="14" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="6" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" s="6" customFormat="1" ht="29" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -708,21 +709,24 @@
       <c r="O1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q1"/>
-      <c r="R1" s="7"/>
-      <c r="S1"/>
+      <c r="R1"/>
+      <c r="S1" s="7"/>
       <c r="T1"/>
+      <c r="U1"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21">
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21">
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21">
       <c r="N4" s="1"/>
     </row>
   </sheetData>

</xml_diff>